<commit_message>
Add support for productItemView for *.docx and *.htm(l)
</commit_message>
<xml_diff>
--- a/files/网站配置.xlsx
+++ b/files/网站配置.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workplace\company_introduce\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDF02D-88B5-4EB0-A47D-7BE8F24AF9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24300" windowHeight="11790" activeTab="5"/>
+    <workbookView xWindow="1665" yWindow="3180" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="142">
   <si>
     <t>为了脚本正常工作，请不要修改本文件名称、工作表名称与红底的单元格！</t>
   </si>
@@ -278,9 +284,6 @@
     <t>/res/img/product1.jpg</t>
   </si>
   <si>
-    <t>产品1号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>产品2号</t>
   </si>
   <si>
@@ -290,9 +293,6 @@
     <t>/res/img/product2.jpg</t>
   </si>
   <si>
-    <t>产品2号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>产品3号</t>
   </si>
   <si>
@@ -302,9 +302,6 @@
     <t>/res/img/product3.jpg</t>
   </si>
   <si>
-    <t>产品3号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>产品4号</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>/res/img/product4.jpg</t>
   </si>
   <si>
-    <t>产品4号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>产品5号</t>
   </si>
   <si>
@@ -326,9 +320,6 @@
     <t>/res/img/product5.jpg</t>
   </si>
   <si>
-    <t>产品5号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>产品6号</t>
   </si>
   <si>
@@ -338,9 +329,6 @@
     <t>/res/img/product6.jpg</t>
   </si>
   <si>
-    <t>产品6号: 随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。\r\n随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。随便写点什么填充一下，到时候全部要替换掉的英文就不写了。</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -471,19 +459,38 @@
   </si>
   <si>
     <t>Simon-Date</t>
+  </si>
+  <si>
+    <t>/res/img/product1.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/res/files/test.html</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/res/files/test.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docx</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,151 +506,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,194 +539,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -857,255 +548,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1121,11 +570,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1133,65 +579,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1478,183 +886,182 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" ht="27" spans="1:16">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="8" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:K10"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A4:P4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:K10"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
@@ -1662,7 +1069,7 @@
     <col min="4" max="4" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1676,7 +1083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1690,7 +1097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1704,7 +1111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1718,7 +1125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1732,7 +1139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1746,7 +1153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1760,7 +1167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1774,7 +1181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1788,7 +1195,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1803,29 +1210,28 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="15.75" customWidth="1"/>
     <col min="3" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1839,7 +1245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1853,7 +1259,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1867,7 +1273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1882,28 +1288,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="6" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1929,7 +1334,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" ht="409.5" spans="1:8">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1949,7 +1354,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1969,7 +1374,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" ht="409.5" spans="1:8">
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1996,32 +1401,32 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 B2:B1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"text,image,mixed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.75" customWidth="1"/>
     <col min="3" max="4" width="23.75" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -2041,7 +1446,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2052,131 +1457,131 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>87</v>
       </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>89</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>91</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.875" customWidth="1"/>
     <col min="2" max="2" width="19.125" customWidth="1"/>
@@ -2184,7 +1589,7 @@
     <col min="4" max="4" width="99.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2198,26 +1603,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -2226,124 +1631,124 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
         <v>109</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>112</v>
       </c>
-      <c r="C5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>115</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>116</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>118</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>115</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>121</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>122</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>124</v>
       </c>
-      <c r="C9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="D11" t="s">
         <v>126</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C12" s="2">
         <v>123456789</v>
@@ -2352,26 +1757,26 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C14" s="2">
         <v>123456789</v>
@@ -2380,36 +1785,36 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s">
         <v>138</v>
       </c>
-      <c r="D15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" t="s">
-        <v>144</v>
-      </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
select default language from broser navagator
</commit_message>
<xml_diff>
--- a/files/网站配置.xlsx
+++ b/files/网站配置.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workplace\company_introduce\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680FBCF4-8F75-4301-94CD-FF7AE8DD0C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961A17AC-9A90-4081-81B7-71AB407C13AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1980" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="164">
   <si>
     <t>为了脚本正常工作，请不要修改本文件名称、工作表名称与红底的单元格！</t>
   </si>
@@ -708,6 +708,26 @@
       </rPr>
       <t>These will display on the blog list page</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blog.banner_img</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"博客"标题图片</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/res/img/banner_about.jpg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/res/img/banner_contact.png</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/res/img/banner_blog.webp</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -808,6 +828,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -819,12 +845,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1139,84 +1159,84 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1226,17 +1246,17 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1246,33 +1266,33 @@
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1293,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1399,7 +1419,7 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -1421,29 +1441,43 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1815,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F299B3A2-7119-4406-B82F-88B989C168FE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1839,10 +1873,10 @@
       <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>155</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1865,10 +1899,10 @@
       <c r="D2" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -1891,10 +1925,10 @@
       <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -1917,10 +1951,10 @@
       <c r="D4" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -1943,10 +1977,10 @@
       <c r="D5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G5" t="s">
@@ -1969,10 +2003,10 @@
       <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G6" t="s">
@@ -1995,10 +2029,10 @@
       <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="8" t="s">
         <v>158</v>
       </c>
       <c r="G7" t="s">

</xml_diff>